<commit_message>
coba.ktr and edit target
</commit_message>
<xml_diff>
--- a/target_sales.xlsx
+++ b/target_sales.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TETRIS_2\Pentaho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repo Proyek\etl-excel-mysql-pentaho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A998DBB-0463-41BE-B135-A40E487AD6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C2878C-7F56-4A9D-A672-9FCD97DB46B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Target Penjualan" sheetId="1" r:id="rId1"/>
+    <sheet name="Sales Target" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>